<commit_message>
Presentation for CEVA collaborators 23-3-2020
</commit_message>
<xml_diff>
--- a/compareOne_checked.xlsx
+++ b/compareOne_checked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Surfdrive\Models_and_Scripts\TransmissionExperiment\TransmissionEstimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D5832-4F2F-433F-804C-1854A08BF7AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD50A4C6-A0B8-4719-814A-470FFA5A6C50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3629" uniqueCount="500">
   <si>
     <t>Group</t>
   </si>
@@ -1556,13 +1556,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1571,39 +1572,9 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1913,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,8 +1977,8 @@
       <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
-        <v>32</v>
+      <c r="H2" s="1">
+        <v>29.25</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -13159,13 +13130,18 @@
     <sortCondition ref="E2:E195"/>
     <sortCondition ref="D2:D195"/>
   </sortState>
+  <conditionalFormatting sqref="F2:S155">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>"&gt;33"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{088979E7-B443-4636-9A24-DB1383914146}">
+          <x14:cfRule type="expression" priority="6" id="{088979E7-B443-4636-9A24-DB1383914146}">
             <xm:f>Reform!E2 =1</xm:f>
             <x14:dxf>
               <fill>
@@ -13178,20 +13154,7 @@
           <xm:sqref>F2:S78</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{444907C5-5CB7-4DB6-97D1-C5E3E4A11F8B}">
-            <xm:f>Reform!F2 =1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>G2:K2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{0B618129-C533-4B5C-9B10-8731DCF9E0E4}">
+          <x14:cfRule type="expression" priority="4" id="{0B618129-C533-4B5C-9B10-8731DCF9E0E4}">
             <xm:f>Reform!E2=1</xm:f>
             <x14:dxf>
               <fill>
@@ -17655,7 +17618,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:R78">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>